<commit_message>
multi graph working with static colors
</commit_message>
<xml_diff>
--- a/VehicleParameters.xlsx
+++ b/VehicleParameters.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11214"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alyssamcpoyle/YawMoment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60D19251-2A43-1542-83B7-DF7E6B1772FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B19D17AE-E4D0-B94F-BDD6-B421D1EB9A6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13580" yWindow="1880" windowWidth="14620" windowHeight="15580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="38">
   <si>
     <t>ParameterName</t>
   </si>
@@ -144,15 +144,6 @@
   </si>
   <si>
     <t>length</t>
-  </si>
-  <si>
-    <t>v</t>
-  </si>
-  <si>
-    <t>velocity</t>
-  </si>
-  <si>
-    <t>m/s</t>
   </si>
   <si>
     <t>vehicleName</t>
@@ -476,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -713,22 +704,8 @@
       <c r="A19" t="s">
         <v>36</v>
       </c>
-      <c r="B19">
-        <v>10</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="B19" t="s">
         <v>37</v>
-      </c>
-      <c r="D19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>